<commit_message>
add new images for settings dialog
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -12,7 +12,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SourceLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
   <si>
     <t xml:space="preserve">CSharp_Is_Love</t>
   </si>
@@ -42,15 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">Du läggs till</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I_Am_Old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I am old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jag är gammal</t>
   </si>
   <si>
     <t xml:space="preserve">Happy</t>
@@ -106,80 +109,80 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1"/>
+    </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Published the extension to windows marketplace
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t xml:space="preserve">Lycklig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cars_Are_Fun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cars are fun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilar är kul</t>
   </si>
 </sst>
 </file>
@@ -184,6 +193,21 @@
       </c>
       <c r="E5"/>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix for only show buttons on the correct file type
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bilar är kul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hund</t>
   </si>
 </sst>
 </file>
@@ -208,6 +214,21 @@
       </c>
       <c r="E6"/>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to support vs 2022
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fågel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love_Is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kärlek är</t>
   </si>
 </sst>
 </file>
@@ -265,6 +274,21 @@
       </c>
       <c r="E9"/>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix for vs mac 2022
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t xml:space="preserve">Kärlek är</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land</t>
   </si>
 </sst>
 </file>
@@ -289,6 +295,21 @@
       </c>
       <c r="E10"/>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add loger for mac
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.sv-SE.resx.xlsx
@@ -5,42 +5,75 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joacimwall/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joacimwall/GitRepos/Visual-studio-multilingual-extension/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA4DBA6-0ED8-C445-9A5D-96DD6988436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCB6B43-9518-B547-BD6B-2EF6D31C4C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Translations" sheetId="1" r:id="rId1"/>
+    <sheet name="Transaltions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>SourceLanguage</t>
-  </si>
-  <si>
-    <t>TargetLanguage</t>
+    <t>Source Language</t>
+  </si>
+  <si>
+    <t>Target Language</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hallå</t>
+  </si>
+  <si>
+    <t>Need review</t>
+  </si>
+  <si>
+    <t>Press_Any_Key_To_Exit</t>
+  </si>
+  <si>
+    <t>Press any key to exit</t>
+  </si>
+  <si>
+    <t>tryck på valfri tangent för att avsluta</t>
+  </si>
+  <si>
+    <t>Enter_Email</t>
+  </si>
+  <si>
+    <t>Enter email please!</t>
+  </si>
+  <si>
+    <t>Ange email tack!</t>
+  </si>
+  <si>
+    <t>Enter_Email_To_Be_The_Next_User_To_Be_Able_To_Login_To_The_Best_Office_System_In_The_World</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
     <t>Lösenord</t>
   </si>
   <si>
-    <t>Need review</t>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Hem</t>
   </si>
   <si>
     <t>Dog</t>
@@ -55,21 +88,18 @@
     <t>Katt</t>
   </si>
   <si>
-    <t>Press_Any_Key_To_Exit</t>
-  </si>
-  <si>
-    <t>Press any key to exit</t>
-  </si>
-  <si>
-    <t>Tryck på valfri tangent för att avsluta</t>
-  </si>
-  <si>
     <t>Bird</t>
   </si>
   <si>
     <t>Fågel</t>
   </si>
   <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Ko</t>
+  </si>
+  <si>
     <t>Love_Is</t>
   </si>
   <si>
@@ -79,12 +109,27 @@
     <t>Kärlek är</t>
   </si>
   <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Hus</t>
+  </si>
+  <si>
     <t>Street</t>
   </si>
   <si>
     <t>Gata</t>
   </si>
   <si>
+    <t>Street_And_House2</t>
+  </si>
+  <si>
+    <t>Street and House and Room. later this day i was so sad that i jumped</t>
+  </si>
+  <si>
+    <t>Gata och Hus och Rum. senare denna dag var jag så ledsen att jag hoppade</t>
+  </si>
+  <si>
     <t>Computer</t>
   </si>
   <si>
@@ -97,34 +142,24 @@
     <t>Kopp</t>
   </si>
   <si>
-    <t>Enter_Email</t>
-  </si>
-  <si>
-    <t>Enter email please!</t>
-  </si>
-  <si>
-    <t>Ange email tack!</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>Hallå</t>
-  </si>
-  <si>
-    <t>Enter_Email_To_Be_The_Next_User_To_Be_Able_To_Login_To_The_Best_Office_System_In_The_World</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Hem</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Hus</t>
+    <t>Read_Instructions</t>
+  </si>
+  <si>
+    <t>Read
+Instructions</t>
+  </si>
+  <si>
+    <t>Läsa
+Instruktioner</t>
+  </si>
+  <si>
+    <t>Nice_Gool_Nice_Shot</t>
+  </si>
+  <si>
+    <t>Nice goal. Nice Shot.</t>
+  </si>
+  <si>
+    <t>Snyggt mål. Snyggt skott.</t>
   </si>
   <si>
     <t>Final</t>
@@ -134,13 +169,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,8 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,33 +517,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -519,49 +559,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -575,105 +615,105 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -684,20 +724,76 @@
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>